<commit_message>
updated publisher and added image tools
</commit_message>
<xml_diff>
--- a/featured-image-sizes.xlsx
+++ b/featured-image-sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnGruber\Documents\gitbit-site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2935AC6-8AF5-4BCA-A893-75BB5332C0B2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4204C246-396A-4B17-A739-A51326A0FD60}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{48066534-DFFA-4914-AF78-CC6D349F34FB}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>height</t>
   </si>
   <si>
     <t>width</t>
+  </si>
+  <si>
+    <t>PPT height</t>
+  </si>
+  <si>
+    <t>PPT width</t>
   </si>
 </sst>
 </file>
@@ -382,44 +388,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5060A9-3B6F-4D4E-9AD1-C6D4B30912E7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>675</v>
       </c>
       <c r="B2">
         <v>1200</v>
       </c>
+      <c r="C2">
+        <v>7.03</v>
+      </c>
+      <c r="D2">
+        <v>12.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>900</v>
       </c>
       <c r="B3">
         <v>1200</v>
       </c>
+      <c r="C3">
+        <v>9.375</v>
+      </c>
+      <c r="D3">
+        <v>12.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1200</v>
       </c>
       <c r="B4">
         <v>1200</v>
+      </c>
+      <c r="C4">
+        <v>12.5</v>
+      </c>
+      <c r="D4">
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>